<commit_message>
PROS-12599 - MARSRU - KPIs PSS 2020
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2018/MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2018/MARS KPIs.xlsx
@@ -17,7 +17,7 @@
     <sheet name="2254" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="golden_shelves" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="survey_answers_translation" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Разбивка по форматам" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="sku_lists" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
@@ -30,11 +30,11 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
@@ -47,6 +47,9 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -58,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="323">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -1213,6 +1216,9 @@
   <si>
     <t xml:space="preserve">DentaStix</t>
   </si>
+  <si>
+    <t xml:space="preserve">SKU List</t>
+  </si>
 </sst>
 </file>
 
@@ -1223,7 +1229,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1274,8 +1280,16 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1291,13 +1305,19 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF33CCCC"/>
+        <bgColor rgb="FF3399FF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3399FF"/>
+        <bgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
   </fills>
@@ -1346,7 +1366,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1519,6 +1539,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1571,7 +1599,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF3399FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF92D050"/>
       <rgbColor rgb="FFFFCC00"/>
@@ -1603,36 +1631,36 @@
   </sheetPr>
   <dimension ref="1:72"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="L73" activeCellId="0" sqref="L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.7408906882591"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="38.9919028340081"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="100.263157894737"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="103.692307692308"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="37.5991902834008"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="22" min="19" style="3" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="24" min="23" style="3" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="3" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="4" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="1" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="42.0485829959514"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="7.88259109311741"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="2" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="22.165991902834"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="3" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="3" width="48.4453441295547"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="3" width="125"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="129.226720647773"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="47.5303643724696"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="3" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="28.9068825910931"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="10.8542510121457"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="4" width="46.7327935222672"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="3" width="26.165991902834"/>
+    <col collapsed="false" hidden="false" max="22" min="19" style="3" width="20.1093117408907"/>
+    <col collapsed="false" hidden="false" max="24" min="23" style="3" width="25.5951417004049"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="3" width="22.165991902834"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="3" width="28.336032388664"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="4" width="24.4534412955466"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="1" width="10.3967611336032"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -49344,7 +49372,7 @@
         <v>155</v>
       </c>
       <c r="L47" s="14" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="M47" s="13" t="s">
         <v>50</v>
@@ -49354,9 +49382,7 @@
       </c>
       <c r="O47" s="0"/>
       <c r="P47" s="14"/>
-      <c r="Q47" s="14" t="s">
-        <v>40</v>
-      </c>
+      <c r="Q47" s="14"/>
       <c r="R47" s="4" t="s">
         <v>156</v>
       </c>
@@ -53562,7 +53588,7 @@
         <v>155</v>
       </c>
       <c r="L51" s="14" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="M51" s="13" t="s">
         <v>50</v>
@@ -53572,9 +53598,7 @@
       </c>
       <c r="O51" s="0"/>
       <c r="P51" s="14"/>
-      <c r="Q51" s="14" t="s">
-        <v>40</v>
-      </c>
+      <c r="Q51" s="14"/>
       <c r="R51" s="14" t="s">
         <v>156</v>
       </c>
@@ -65361,7 +65385,9 @@
       <c r="K66" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="L66" s="4"/>
+      <c r="L66" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="M66" s="2" t="s">
         <v>50</v>
       </c>
@@ -65474,7 +65500,9 @@
       <c r="K68" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="L68" s="4"/>
+      <c r="L68" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="M68" s="2" t="s">
         <v>50</v>
       </c>
@@ -65527,7 +65555,9 @@
       <c r="K69" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="L69" s="4"/>
+      <c r="L69" s="4" t="s">
+        <v>70</v>
+      </c>
       <c r="M69" s="2" t="s">
         <v>50</v>
       </c>
@@ -65717,20 +65747,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="43" width="18.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="29.4777327935223"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="43" width="11.1983805668016"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="28.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -65746,16 +65789,16 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="26" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="46.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="12.7975708502024"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="25" width="13.1417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="46.6194331983806"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="26" width="13.4817813765182"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65853,11 +65896,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="37.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="26" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="46.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="26" width="13.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="26" width="13.0242914979757"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="26" width="46.6194331983806"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="26" width="13.4817813765182"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -65954,11 +65997,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="65.8785425101215"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7975708502024"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="82.0404858299595"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7935222672065"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66083,11 +66126,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="67.2712550607288"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="33" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="33" width="32.336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="33" width="13.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="33" width="83.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="33" width="45.3603238866397"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="33" width="13.4817813765182"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -66212,9 +66255,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="55.4858299595142"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="25" width="10.7125506072875"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="25" width="69.1255060728745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="25" width="46.6194331983806"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="25" width="13.1417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="34" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -66321,15 +66364,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="39.6356275303644"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.0323886639676"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="64.2145748987854"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="49.3603238866397"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="45.3603238866397"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="28.5668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="35.0769230769231"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.5668016194332"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3967611336032"/>
   </cols>
   <sheetData>
     <row r="1" s="36" customFormat="true" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -68802,11 +68845,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.5951417004049"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6801619433198"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -68851,10 +68894,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="16.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.0769230769231"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="22.2793522267206"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.3967611336032"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>